<commit_message>
New docking path. GNSS HW Reset command added. MOONLIGHT_DOCKING_SPEED added. Stop immediately during docking.
</commit_message>
<xml_diff>
--- a/amcp/DockPoints.xlsx
+++ b/amcp/DockPoints.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>dx1 =  2.78  #  3.14</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>Einfahrt - Startpunkt (Einfahrtrichtung)</t>
+  </si>
+  <si>
+    <t>Startpunkt</t>
+  </si>
+  <si>
+    <t>Zwischenwert</t>
+  </si>
+  <si>
+    <t>Einfahrt</t>
+  </si>
+  <si>
+    <t>Endpunkt</t>
+  </si>
+  <si>
+    <t>Verschiebung nach links 10 cm</t>
   </si>
 </sst>
 </file>
@@ -468,16 +483,16 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="5" width="11.42578125" style="3"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="20.1328125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="48.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.3984375" style="1"/>
+    <col min="5" max="5" width="11.3984375" style="3"/>
+    <col min="6" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,17 +652,77 @@
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2">
+        <f>-D12*E14</f>
+        <v>-7.8985231415738558E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <f>C12*E14</f>
+        <v>-6.1329709099279366E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2">
+        <f>C5+C$14</f>
+        <v>3.3610147685842615</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" ref="D16:D19" si="0">D5+D$14</f>
+        <v>-1.5013297090992792</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:D17" si="1">C6+C$14</f>
+        <v>3.0310147685842614</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.0763297090992792</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:D18" si="2">C7+C$14</f>
+        <v>2.7010147685842614</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.65132970909927934</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" ref="C19:D19" si="3">C8+C$14</f>
+        <v>2.4556959321871439</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.33538878343632511</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +737,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -674,7 +749,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New docking path. GNSS HW Reset command added. MOONLIGHT_DOCKING_SPEED added.
</commit_message>
<xml_diff>
--- a/amcp/DockPoints.xlsx
+++ b/amcp/DockPoints.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>dx1 =  2.78  #  3.14</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>Einfahrt - Startpunkt (Einfahrtrichtung)</t>
+  </si>
+  <si>
+    <t>Startpunkt</t>
+  </si>
+  <si>
+    <t>Zwischenwert</t>
+  </si>
+  <si>
+    <t>Einfahrt</t>
+  </si>
+  <si>
+    <t>Endpunkt</t>
+  </si>
+  <si>
+    <t>Verschiebung nach links 10 cm</t>
   </si>
 </sst>
 </file>
@@ -468,16 +483,16 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="5" width="11.42578125" style="3"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="20.1328125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="48.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.3984375" style="1"/>
+    <col min="5" max="5" width="11.3984375" style="3"/>
+    <col min="6" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,17 +652,77 @@
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2">
+        <f>-D12*E14</f>
+        <v>-7.8985231415738558E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <f>C12*E14</f>
+        <v>-6.1329709099279366E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2">
+        <f>C5+C$14</f>
+        <v>3.3610147685842615</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" ref="D16:D19" si="0">D5+D$14</f>
+        <v>-1.5013297090992792</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:D17" si="1">C6+C$14</f>
+        <v>3.0310147685842614</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.0763297090992792</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:D18" si="2">C7+C$14</f>
+        <v>2.7010147685842614</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.65132970909927934</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" ref="C19:D19" si="3">C8+C$14</f>
+        <v>2.4556959321871439</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.33538878343632511</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +737,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -674,7 +749,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>